<commit_message>
added final project after updating
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Payal\QA Classes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium_WorkSpace\FreeCRMTest\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D90F416E-0C4B-49B8-9B9A-36D4BA289680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E674AA-A1BF-4BA4-B158-3173012775A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1F75721-1A45-4FA8-B302-2AE04C75A2B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E1F75721-1A45-4FA8-B302-2AE04C75A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="deals" sheetId="2" r:id="rId2"/>
+    <sheet name="Calendar" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>firstname</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>Contact</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Morning Session</t>
+  </si>
+  <si>
+    <t>Afternon Session</t>
+  </si>
+  <si>
+    <t>Evening session</t>
+  </si>
+  <si>
+    <t>Important</t>
+  </si>
+  <si>
+    <t>Oportunity</t>
+  </si>
+  <si>
+    <t>Optional</t>
   </si>
 </sst>
 </file>
@@ -433,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC856D40-4E05-4C85-BDD2-E956551F9D45}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,12 +511,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B1EAAF-4EFA-4BDD-A1DA-39E1BA12D35B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>